<commit_message>
MaxAnalysisLevel 글로벌 상수 추가
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3759510-6153-4E27-BF2B-67192265574C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0A8D05-DB01-4A60-BB11-0651DD0BD326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id|String</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>FirstGoldBox</t>
+  </si>
+  <si>
+    <t>MaxAnalysisLevel</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5000017-DE11-4746-A50F-C02BCCA15C78}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -587,6 +590,14 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TimeSecToGetOneSpin => TimeSecToGetOneEnergy 로 글로벌 상수 이름 변경
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A2D66D-C1DC-4534-A18B-6F09F93EE12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72F88E5-BA9B-4761-8600-8152F2C6A602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>MaxPlayerLevel</t>
   </si>
   <si>
-    <t>TimeSecToGetOneSpin</t>
-  </si>
-  <si>
     <t>SubLevelFightValueLine1</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>MaxGuideQuestId</t>
+  </si>
+  <si>
+    <t>TimeSecToGetOneEnergy</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>400</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>576</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -547,7 +547,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>50</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>2000</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>110</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>20</v>

</xml_diff>

<commit_message>
글로벌 상수 제거 Bet3Diamonds Bet3Spins Bet3Tickets Bet1Event Bet2Events Bet3Events
글로벌 상수 추가
GachaEnergy
Gacha1Event
Gacha2Events
Gacha3Events
Gacha1BrokenEnergy
Gacha2BrokenEnergys

베팅 => 뽑기로 변경하면서 글로벌 상수 수정 엑셀만 적용한다
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72F88E5-BA9B-4761-8600-8152F2C6A602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB19556-FEEE-4588-81C8-072533A36B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -54,24 +54,6 @@
     <t>SubLevelFightValueLine3</t>
   </si>
   <si>
-    <t>Bet3Diamonds</t>
-  </si>
-  <si>
-    <t>Bet3Spins</t>
-  </si>
-  <si>
-    <t>Bet3Tickets</t>
-  </si>
-  <si>
-    <t>Bet1Event</t>
-  </si>
-  <si>
-    <t>Bet2Events</t>
-  </si>
-  <si>
-    <t>Bet3Events</t>
-  </si>
-  <si>
     <t>MaxStage</t>
   </si>
   <si>
@@ -91,6 +73,24 @@
   </si>
   <si>
     <t>TimeSecToGetOneEnergy</t>
+  </si>
+  <si>
+    <t>GachaEnergy</t>
+  </si>
+  <si>
+    <t>Gacha1Event</t>
+  </si>
+  <si>
+    <t>Gacha2Events</t>
+  </si>
+  <si>
+    <t>Gacha3Events</t>
+  </si>
+  <si>
+    <t>Gacha1BrokenEnergy</t>
+  </si>
+  <si>
+    <t>Gacha2BrokenEnergys</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>400</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>576</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -531,47 +531,47 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>50</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>2000</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>110</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>20</v>

</xml_diff>

<commit_message>
Gacha3BrokenEnergys 추가하고 Gacha3Events 의 값을 10 => 9 로 수정
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF87A628-C594-4928-BF47-403A191E23A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0372758-2E27-425A-AE8F-D1F1C7B37480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-26850" yWindow="1935" windowWidth="13515" windowHeight="14265" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>id|String</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>MaxBrokenEnergy</t>
+  </si>
+  <si>
+    <t>Gacha3BrokenEnergys</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5000017-DE11-4746-A50F-C02BCCA15C78}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -553,7 +556,7 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -574,49 +577,57 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>1000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
-        <v>110</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18">
-        <v>20</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>2000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MaxTotalSkillLevel => MaxTotalSpellLevel 인트 상수 변경 수치를 임시 10 으로 변경
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4B32BD-2848-404C-8723-90319DD3C118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F216F7D9-C604-41C5-BE1B-A5A50E75C707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="495" windowWidth="18915" windowHeight="14805" activeTab="1" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>Gacha3BrokenEnergys</t>
   </si>
   <si>
-    <t>MaxTotalSkillLevel</t>
-  </si>
-  <si>
     <t>value|String</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>1, 3, 5</t>
+  </si>
+  <si>
+    <t>MaxTotalSpellLevel</t>
   </si>
 </sst>
 </file>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5000017-DE11-4746-A50F-C02BCCA15C78}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -652,10 +652,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -668,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED29560-8EF7-45A2-9D29-FD68F5C70330}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -681,23 +681,23 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
펫 관련 상수 추가 MaxPetCountStep PetSaleGivenTime PetSaleCoolTime
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DF45B2-148F-4FAA-B640-942401A5E167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6483BF-2FFE-4CEC-A88D-2E9804459332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-28800" yWindow="780" windowWidth="28800" windowHeight="12885" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>id|String</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>PetPassHeartCount</t>
+  </si>
+  <si>
+    <t>MaxPetCountStep</t>
+  </si>
+  <si>
+    <t>PetSaleGivenTime</t>
+  </si>
+  <si>
+    <t>PetSaleCoolTime</t>
   </si>
 </sst>
 </file>
@@ -524,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5000017-DE11-4746-A50F-C02BCCA15C78}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -769,58 +778,82 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>172800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
글로벌 상수 TimeSecToGetOneTicket 960 추가
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0CA880-B9AC-46A8-A172-8BAA6904A0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4DB498-795B-428E-B245-5EFDDA7252CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>id|String</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>MaxBossDefense</t>
+  </si>
+  <si>
+    <t>TimeSecToGetOneTicket</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5000017-DE11-4746-A50F-C02BCCA15C78}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -673,159 +676,159 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>960</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>2000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>259200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>259200</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B23">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -833,191 +836,191 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B31">
-        <v>300</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B32">
-        <v>9</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B33">
-        <v>1209600</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1209600</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <v>2419200</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>2419200</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>66</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>86400</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45">
-        <v>172800</v>
+        <v>86400</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46">
-        <v>200</v>
+        <v>172800</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49">
         <v>10</v>
@@ -1025,23 +1028,23 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52">
         <v>5</v>
@@ -1049,15 +1052,15 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -1065,7 +1068,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -1073,15 +1076,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57">
         <v>16</v>
@@ -1089,89 +1092,97 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B58">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B62">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B64">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B66">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67">
-        <v>1200</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>61</v>
       </c>
-      <c r="B68">
+      <c r="B69">
         <v>3330</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BossBattleDailyCount 5 => 3 변경
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27510419-3843-4B26-A30B-1C21C3FB9273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1604290E-E367-458D-AAB3-01971BC1F09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2670" windowWidth="24240" windowHeight="13140" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -1192,7 +1192,7 @@
         <v>74</v>
       </c>
       <c r="B63">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
디프값 100 => 10
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BD28B2-818F-4736-957E-EE98BF66FDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB403DA5-CBE2-475D-A1C7-D4395C34E183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2670" windowWidth="24240" windowHeight="13140" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
@@ -1136,7 +1136,7 @@
         <v>101</v>
       </c>
       <c r="B53">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SpellGachaLevelAccumulatedCount 글로벌 상수 스트링 추가
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D18B9A-5193-44BA-95C4-85BF3894D1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7706674C-AE11-4F8E-8CDA-2F26B538C033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2670" windowWidth="24240" windowHeight="13140" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
+    <workbookView xWindow="28680" yWindow="2670" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>id|String</t>
   </si>
@@ -341,6 +341,12 @@
   </si>
   <si>
     <t>PetStarDiff100</t>
+  </si>
+  <si>
+    <t>SpellGachaLevelAccumulatedCount</t>
+  </si>
+  <si>
+    <t>0, 10, 45, 190, 780, 2415, 5950, 10950, 15950, 21950, 28950, 36950, 45950, 54950</t>
   </si>
 </sst>
 </file>
@@ -706,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5000017-DE11-4746-A50F-C02BCCA15C78}">
   <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1467,11 +1473,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED29560-8EF7-45A2-9D29-FD68F5C70330}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1505,17 +1509,25 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
450 => 1300 밸런싱 조정
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85B1DDA-35A3-4702-88D8-A7882902D939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B679FA50-EC9F-4C2B-AF80-A8AF928847AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2670" windowWidth="24240" windowHeight="13140" xr2:uid="{385C27BB-68F4-4CA4-9DDE-8BDC8C2EA378}"/>
   </bookViews>
@@ -1473,7 +1473,7 @@
         <v>104</v>
       </c>
       <c r="B94">
-        <v>450</v>
+        <v>1300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>